<commit_message>
Añadida columna 'excluido' en la hoja los recursos, así como su funcionalidad. También se han adaptado los ficheros de configuracón de prueba, para evitar problemas en las pruebas unitarias.
</commit_message>
<xml_diff>
--- a/EjerciciosLog/PrezConfig.xlsx
+++ b/EjerciciosLog/PrezConfig.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sal8b\OneDrive\Escritorio\LibreriaMoodleAnalisis\EjerciciosLog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503BA9F5-79B8-45B9-A743-8795060E4ED7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35EE866-9EFC-4B4E-B6C8-73F2E44AC918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
     <sheet name="Recursos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Nombre completo del usuario</t>
   </si>
@@ -113,7 +113,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -174,7 +177,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -216,7 +219,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,9 +251,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -282,6 +303,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -460,9 +499,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -538,29 +580,35 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="48.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -568,7 +616,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -576,7 +624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -584,7 +632,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -592,7 +640,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -600,7 +648,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -608,7 +656,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -617,6 +665,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reformulación de Prez, Maadle y clase de test para identificar a su recurso por su ID.
</commit_message>
<xml_diff>
--- a/EjerciciosLog/PrezConfig.xlsx
+++ b/EjerciciosLog/PrezConfig.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sal8b\OneDrive\Escritorio\LibreriaMoodleAnalisis\EjerciciosLog\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35EE866-9EFC-4B4E-B6C8-73F2E44AC918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
     <sheet name="Recursos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Nombre completo del usuario</t>
   </si>
@@ -71,38 +65,35 @@
     <t>Contexto del evento</t>
   </si>
   <si>
+    <t>IDRecurso</t>
+  </si>
+  <si>
     <t>Alias</t>
   </si>
   <si>
-    <t>Curso: G000 - Curso de Testing - Curso 2018-2019</t>
+    <t>Foro: Noticias de clase</t>
+  </si>
+  <si>
+    <t>Carpeta: Exámenes</t>
   </si>
   <si>
     <t>Carpeta: Recursos del Alumnado</t>
   </si>
   <si>
+    <t>Carpeta: Papeleo</t>
+  </si>
+  <si>
+    <t>Tarea: Entrega inicial</t>
+  </si>
+  <si>
     <t>Carpeta: Entrega inicial</t>
-  </si>
-  <si>
-    <t>Tarea: Entrega inicial</t>
-  </si>
-  <si>
-    <t>Carpeta: Papeleo</t>
-  </si>
-  <si>
-    <t>Foro: Noticias de clase</t>
-  </si>
-  <si>
-    <t>Carpeta: Exámenes</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,19 +156,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -219,7 +202,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,27 +234,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,24 +268,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -496,17 +443,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,67 +461,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -585,19 +532,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="48.7109375" customWidth="1"/>
+    <col min="1" max="3" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -605,62 +551,97 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>5000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>5002</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>5011</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>5012</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>5013</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>5014</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8">
+        <v>5015</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9">
+        <v>5016</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>